<commit_message>
Editar y visualizar caratula
Se terminaron los modulos de edición y vista de los datos de caratulas /layout generados.
</commit_message>
<xml_diff>
--- a/winAsimilados/Resources/Formato_Masivo_Empleados.xlsx
+++ b/winAsimilados/Resources/Formato_Masivo_Empleados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aespejel\source\repos\winAsimilados\winAsimilados\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFD9A5F-AC80-449D-9145-F0BE1CC34CD8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE3177D-7890-412A-980C-B5418990340A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{669BB77A-E265-42D7-8B1F-40247EB15B12}"/>
   </bookViews>
@@ -1445,10 +1445,10 @@
     <t>SCOTIABANK</t>
   </si>
   <si>
-    <t>GRUPO ARYVE</t>
-  </si>
-  <si>
     <t>E00132</t>
+  </si>
+  <si>
+    <t>CONSTRUCCIONES ARYVE SA DE CV</t>
   </si>
 </sst>
 </file>
@@ -1954,10 +1954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF2366B-8682-479D-85C8-42D73AA8D484}">
-  <dimension ref="A1:L92"/>
+  <dimension ref="A1:L93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="D3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1970,7 +1970,7 @@
     <col min="7" max="7" width="20.140625" style="6" customWidth="1"/>
     <col min="8" max="8" width="28.42578125" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+    <col min="10" max="10" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2039,68 +2039,45 @@
         <v>466</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
-        <v>314</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="H3" s="7">
-        <v>1</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>472</v>
-      </c>
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H4" s="7">
         <v>1</v>
@@ -2109,103 +2086,103 @@
         <v>466</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H5" s="7">
         <v>1</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H6" s="7">
         <v>1</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H7" s="7">
         <v>1</v>
@@ -2214,173 +2191,173 @@
         <v>466</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
+        <v>318</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="H8" s="7">
+        <v>1</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
         <v>319</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C9" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D9" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="10" t="s">
+      <c r="E9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G9" s="13" t="s">
         <v>298</v>
       </c>
-      <c r="H8" s="7">
-        <v>1</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="H9" s="7">
+        <v>1</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
         <v>320</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C10" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D10" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="E10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G10" s="13" t="s">
         <v>300</v>
       </c>
-      <c r="H9" s="7">
-        <v>1</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <v>321</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>301</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>302</v>
-      </c>
       <c r="H10" s="7">
         <v>1</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="H11" s="7">
         <v>1</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H12" s="7">
         <v>1</v>
@@ -2389,33 +2366,33 @@
         <v>466</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H13" s="7">
         <v>1</v>
@@ -2424,33 +2401,33 @@
         <v>466</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H14" s="7">
         <v>1</v>
@@ -2459,33 +2436,33 @@
         <v>466</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="H15" s="7">
         <v>1</v>
@@ -2494,33 +2471,33 @@
         <v>466</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K15" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="H16" s="7">
         <v>1</v>
@@ -2529,33 +2506,33 @@
         <v>466</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H17" s="7">
         <v>1</v>
@@ -2564,33 +2541,33 @@
         <v>466</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H18" s="7">
         <v>1</v>
@@ -2599,104 +2576,104 @@
         <v>466</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
+        <v>329</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="H19" s="7">
+        <v>1</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
         <v>330</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B20" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D20" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="10" t="s">
+      <c r="E20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G20" s="13" t="s">
         <v>320</v>
       </c>
-      <c r="H19" s="7">
-        <v>1</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J19" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K19" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
+      <c r="H20" s="7">
+        <v>1</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
         <v>331</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B21" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C21" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D21" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="10" t="s">
+      <c r="E21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="10" t="s">
         <v>321</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G21" s="13" t="s">
         <v>322</v>
       </c>
-      <c r="H20" s="7">
-        <v>1</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J20" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K20" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
-        <v>332</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>323</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>324</v>
-      </c>
       <c r="H21" s="7">
         <v>1</v>
       </c>
@@ -2704,33 +2681,33 @@
         <v>466</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H22" s="7">
         <v>1</v>
@@ -2739,33 +2716,33 @@
         <v>466</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K22" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="H23" s="7">
         <v>1</v>
@@ -2774,33 +2751,33 @@
         <v>466</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H24" s="7">
         <v>1</v>
@@ -2809,33 +2786,33 @@
         <v>466</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K24" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="H25" s="7">
         <v>1</v>
@@ -2844,33 +2821,33 @@
         <v>466</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H26" s="7">
         <v>1</v>
@@ -2879,174 +2856,174 @@
         <v>466</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K26" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
+        <v>337</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="H27" s="7">
+        <v>1</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K27" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
         <v>338</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B28" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C28" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D28" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="10" t="s">
+      <c r="E28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="10" t="s">
         <v>335</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G28" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="H27" s="7">
-        <v>1</v>
-      </c>
-      <c r="I27" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J27" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K27" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
+      <c r="H28" s="7">
+        <v>1</v>
+      </c>
+      <c r="I28" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K28" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
         <v>339</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B29" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C29" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D29" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="10" t="s">
+      <c r="E29" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="G29" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="H28" s="7">
-        <v>1</v>
-      </c>
-      <c r="I28" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J28" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K28" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+      <c r="H29" s="7">
+        <v>1</v>
+      </c>
+      <c r="I29" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="J29" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K29" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
         <v>340</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B30" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C30" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D30" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="10" t="s">
+      <c r="E30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="10" t="s">
         <v>339</v>
       </c>
-      <c r="G29" s="13" t="s">
+      <c r="G30" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="H29" s="7">
-        <v>1</v>
-      </c>
-      <c r="I29" s="14" t="s">
+      <c r="H30" s="7">
+        <v>1</v>
+      </c>
+      <c r="I30" s="14" t="s">
         <v>468</v>
       </c>
-      <c r="J29" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K29" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
+      <c r="J30" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K30" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
         <v>341</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B31" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C31" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D31" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F30" s="10" t="s">
+      <c r="E31" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="G30" s="13" t="s">
+      <c r="G31" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="H30" s="7">
-        <v>1</v>
-      </c>
-      <c r="I30" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J30" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K30" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
-        <v>342</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>343</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>344</v>
-      </c>
       <c r="H31" s="7">
         <v>1</v>
       </c>
@@ -3054,33 +3031,33 @@
         <v>466</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K31" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
+        <v>342</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="10" t="s">
         <v>343</v>
       </c>
-      <c r="B32" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>345</v>
-      </c>
       <c r="G32" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H32" s="7">
         <v>1</v>
@@ -3089,103 +3066,103 @@
         <v>466</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K32" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H33" s="7">
         <v>1</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K33" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H34" s="7">
         <v>1</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K34" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="H35" s="7">
         <v>1</v>
@@ -3194,33 +3171,33 @@
         <v>466</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K35" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H36" s="7">
         <v>1</v>
@@ -3229,33 +3206,33 @@
         <v>466</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K36" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="H37" s="7">
         <v>1</v>
@@ -3264,33 +3241,33 @@
         <v>466</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K37" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="H38" s="7">
         <v>1</v>
@@ -3299,33 +3276,33 @@
         <v>466</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K38" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="H39" s="7">
         <v>1</v>
@@ -3334,103 +3311,103 @@
         <v>466</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K39" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H40" s="7">
         <v>1</v>
       </c>
       <c r="I40" s="14" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K40" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H41" s="7">
         <v>1</v>
       </c>
       <c r="I41" s="14" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K41" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H42" s="7">
         <v>1</v>
@@ -3439,33 +3416,33 @@
         <v>466</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K42" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H43" s="7">
         <v>1</v>
@@ -3474,174 +3451,174 @@
         <v>466</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K43" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
+        <v>354</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="G44" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="H44" s="7">
+        <v>1</v>
+      </c>
+      <c r="I44" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K44" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="9">
         <v>355</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B45" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C45" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D45" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="E44" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F44" s="10" t="s">
+      <c r="E45" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="10" t="s">
         <v>369</v>
       </c>
-      <c r="G44" s="13" t="s">
+      <c r="G45" s="13" t="s">
         <v>370</v>
       </c>
-      <c r="H44" s="7">
-        <v>1</v>
-      </c>
-      <c r="I44" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J44" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K44" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="9">
+      <c r="H45" s="7">
+        <v>1</v>
+      </c>
+      <c r="I45" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="J45" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K45" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="9">
         <v>356</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B46" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C46" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D46" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="E45" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F45" s="10" t="s">
+      <c r="E46" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="G45" s="13" t="s">
+      <c r="G46" s="13" t="s">
         <v>372</v>
       </c>
-      <c r="H45" s="7">
-        <v>1</v>
-      </c>
-      <c r="I45" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J45" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K45" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="9">
+      <c r="H46" s="7">
+        <v>1</v>
+      </c>
+      <c r="I46" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="J46" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K46" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="9">
         <v>357</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B47" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C47" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D47" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="E46" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F46" s="10" t="s">
+      <c r="E47" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="10" t="s">
         <v>373</v>
       </c>
-      <c r="G46" s="13" t="s">
+      <c r="G47" s="13" t="s">
         <v>374</v>
       </c>
-      <c r="H46" s="7">
-        <v>1</v>
-      </c>
-      <c r="I46" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J46" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K46" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="9">
+      <c r="H47" s="7">
+        <v>1</v>
+      </c>
+      <c r="I47" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="J47" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K47" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="9">
         <v>358</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B48" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C48" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="D48" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="E47" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F47" s="10" t="s">
+      <c r="E48" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="10" t="s">
         <v>375</v>
       </c>
-      <c r="G47" s="13" t="s">
+      <c r="G48" s="13" t="s">
         <v>376</v>
       </c>
-      <c r="H47" s="7">
-        <v>1</v>
-      </c>
-      <c r="I47" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J47" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K47" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="9">
-        <v>359</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F48" s="10" t="s">
-        <v>377</v>
-      </c>
-      <c r="G48" s="13" t="s">
-        <v>378</v>
-      </c>
       <c r="H48" s="7">
         <v>1</v>
       </c>
@@ -3649,33 +3626,33 @@
         <v>466</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K48" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="H49" s="7">
         <v>1</v>
@@ -3684,33 +3661,33 @@
         <v>466</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K49" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G50" s="13" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H50" s="7">
         <v>1</v>
@@ -3719,33 +3696,33 @@
         <v>466</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K50" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G51" s="13" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H51" s="7">
         <v>1</v>
@@ -3754,33 +3731,33 @@
         <v>466</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K51" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H52" s="7">
         <v>1</v>
@@ -3789,33 +3766,33 @@
         <v>466</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K52" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G53" s="13" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="H53" s="7">
         <v>1</v>
@@ -3824,33 +3801,33 @@
         <v>466</v>
       </c>
       <c r="J53" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K53" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="H54" s="7">
         <v>1</v>
@@ -3859,33 +3836,33 @@
         <v>466</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K54" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H55" s="7">
         <v>1</v>
@@ -3894,33 +3871,33 @@
         <v>466</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K55" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G56" s="13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="H56" s="7">
         <v>1</v>
@@ -3929,33 +3906,33 @@
         <v>466</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K56" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="G57" s="13" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H57" s="7">
         <v>1</v>
@@ -3964,33 +3941,33 @@
         <v>466</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K57" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="9">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="G58" s="13" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H58" s="7">
         <v>1</v>
@@ -3999,33 +3976,33 @@
         <v>466</v>
       </c>
       <c r="J58" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K58" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="9">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="G59" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H59" s="7">
         <v>1</v>
@@ -4034,33 +4011,33 @@
         <v>466</v>
       </c>
       <c r="J59" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K59" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="9">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F60" s="10" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="G60" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H60" s="7">
         <v>1</v>
@@ -4069,33 +4046,33 @@
         <v>466</v>
       </c>
       <c r="J60" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K60" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="9">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="G61" s="13" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H61" s="7">
         <v>1</v>
@@ -4104,33 +4081,33 @@
         <v>466</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K61" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="9">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="G62" s="13" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H62" s="7">
         <v>1</v>
@@ -4139,33 +4116,33 @@
         <v>466</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K62" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="9">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="G63" s="13" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="H63" s="7">
         <v>1</v>
@@ -4174,33 +4151,33 @@
         <v>466</v>
       </c>
       <c r="J63" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K63" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="G64" s="13" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="H64" s="7">
         <v>1</v>
@@ -4209,314 +4186,314 @@
         <v>466</v>
       </c>
       <c r="J64" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K64" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="9">
+        <v>375</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>409</v>
+      </c>
+      <c r="G65" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="H65" s="7">
+        <v>1</v>
+      </c>
+      <c r="I65" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="J65" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K65" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="9">
         <v>376</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="B66" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C66" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="D65" s="12" t="s">
+      <c r="D66" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="E65" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F65" s="10" t="s">
+      <c r="E66" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66" s="10" t="s">
         <v>411</v>
       </c>
-      <c r="G65" s="13" t="s">
+      <c r="G66" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="H65" s="7">
-        <v>1</v>
-      </c>
-      <c r="I65" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J65" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K65" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="9">
+      <c r="H66" s="7">
+        <v>1</v>
+      </c>
+      <c r="I66" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="J66" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K66" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A67" s="9">
         <v>377</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B67" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C66" s="11" t="s">
+      <c r="C67" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="D66" s="12" t="s">
+      <c r="D67" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="E66" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F66" s="10" t="s">
+      <c r="E67" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="G66" s="13" t="s">
+      <c r="G67" s="13" t="s">
         <v>414</v>
       </c>
-      <c r="H66" s="7">
-        <v>1</v>
-      </c>
-      <c r="I66" s="14" t="s">
+      <c r="H67" s="7">
+        <v>1</v>
+      </c>
+      <c r="I67" s="14" t="s">
         <v>467</v>
       </c>
-      <c r="J66" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K66" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="9">
-        <v>378</v>
-      </c>
-      <c r="B67" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C67" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="D67" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F67" s="10" t="s">
-        <v>415</v>
-      </c>
-      <c r="G67" s="13" t="s">
-        <v>416</v>
-      </c>
-      <c r="H67" s="7">
-        <v>1</v>
-      </c>
-      <c r="I67" s="14" t="s">
-        <v>466</v>
-      </c>
       <c r="J67" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K67" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="9">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F68" s="10" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="G68" s="13" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="H68" s="7">
         <v>1</v>
       </c>
       <c r="I68" s="14" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J68" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K68" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="9">
+        <v>379</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="G69" s="13" t="s">
+        <v>418</v>
+      </c>
+      <c r="H69" s="7">
+        <v>1</v>
+      </c>
+      <c r="I69" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="J69" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K69" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="9">
         <v>380</v>
       </c>
-      <c r="B69" s="10" t="s">
+      <c r="B70" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C69" s="11" t="s">
+      <c r="C70" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="D69" s="12" t="s">
+      <c r="D70" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="E69" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F69" s="10" t="s">
+      <c r="E70" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F70" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="G69" s="13" t="s">
+      <c r="G70" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="H69" s="7">
-        <v>1</v>
-      </c>
-      <c r="I69" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J69" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K69" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="9">
+      <c r="H70" s="7">
+        <v>1</v>
+      </c>
+      <c r="I70" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="J70" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K70" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A71" s="9">
         <v>381</v>
       </c>
-      <c r="B70" s="10" t="s">
+      <c r="B71" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C70" s="11" t="s">
+      <c r="C71" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="D70" s="12" t="s">
+      <c r="D71" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="E70" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F70" s="10" t="s">
+      <c r="E71" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F71" s="10" t="s">
         <v>421</v>
       </c>
-      <c r="G70" s="13" t="s">
+      <c r="G71" s="13" t="s">
         <v>422</v>
       </c>
-      <c r="H70" s="7">
-        <v>1</v>
-      </c>
-      <c r="I70" s="14" t="s">
+      <c r="H71" s="7">
+        <v>1</v>
+      </c>
+      <c r="I71" s="14" t="s">
         <v>470</v>
       </c>
-      <c r="J70" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K70" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="9">
+      <c r="J71" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K71" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="9">
         <v>382</v>
       </c>
-      <c r="B71" s="10" t="s">
+      <c r="B72" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="C72" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="D71" s="12" t="s">
+      <c r="D72" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="E71" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F71" s="10" t="s">
+      <c r="E72" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F72" s="10" t="s">
         <v>423</v>
       </c>
-      <c r="G71" s="13" t="s">
+      <c r="G72" s="13" t="s">
         <v>424</v>
       </c>
-      <c r="H71" s="7">
-        <v>1</v>
-      </c>
-      <c r="I71" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J71" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K71" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="9">
+      <c r="H72" s="7">
+        <v>1</v>
+      </c>
+      <c r="I72" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="J72" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K72" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A73" s="9">
         <v>383</v>
       </c>
-      <c r="B72" s="10" t="s">
+      <c r="B73" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C72" s="11" t="s">
+      <c r="C73" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="D72" s="12" t="s">
+      <c r="D73" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="E72" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F72" s="10" t="s">
+      <c r="E73" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F73" s="10" t="s">
         <v>425</v>
       </c>
-      <c r="G72" s="13" t="s">
+      <c r="G73" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="H72" s="7">
-        <v>1</v>
-      </c>
-      <c r="I72" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J72" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K72" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="9">
-        <v>384</v>
-      </c>
-      <c r="B73" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C73" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="D73" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F73" s="10" t="s">
-        <v>427</v>
-      </c>
-      <c r="G73" s="13" t="s">
-        <v>428</v>
-      </c>
       <c r="H73" s="7">
         <v>1</v>
       </c>
@@ -4524,33 +4501,33 @@
         <v>466</v>
       </c>
       <c r="J73" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K73" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="9">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F74" s="10" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="G74" s="13" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H74" s="7">
         <v>1</v>
@@ -4559,103 +4536,103 @@
         <v>466</v>
       </c>
       <c r="J74" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K74" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="9">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F75" s="10" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="G75" s="13" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H75" s="7">
         <v>1</v>
       </c>
       <c r="I75" s="14" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="J75" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K75" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="9">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="G76" s="13" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="H76" s="7">
         <v>1</v>
       </c>
       <c r="I76" s="14" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="J76" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K76" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="9">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F77" s="10" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="G77" s="13" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H77" s="7">
         <v>1</v>
@@ -4664,33 +4641,33 @@
         <v>466</v>
       </c>
       <c r="J77" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K77" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="9">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F78" s="10" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="G78" s="13" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H78" s="7">
         <v>1</v>
@@ -4699,33 +4676,33 @@
         <v>466</v>
       </c>
       <c r="J78" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K78" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="9">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F79" s="10" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="G79" s="13" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H79" s="7">
         <v>1</v>
@@ -4734,33 +4711,33 @@
         <v>466</v>
       </c>
       <c r="J79" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K79" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="9">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D80" s="12" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F80" s="10" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="G80" s="13" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="H80" s="7">
         <v>1</v>
@@ -4769,139 +4746,139 @@
         <v>466</v>
       </c>
       <c r="J80" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K80" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
+        <v>391</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="D81" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F81" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="G81" s="13" t="s">
+        <v>442</v>
+      </c>
+      <c r="H81" s="7">
+        <v>1</v>
+      </c>
+      <c r="I81" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="J81" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K81" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" s="9">
         <v>392</v>
       </c>
-      <c r="B81" s="10" t="s">
+      <c r="B82" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C81" s="11" t="s">
+      <c r="C82" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="D81" s="12" t="s">
+      <c r="D82" s="12" t="s">
         <v>262</v>
       </c>
-      <c r="E81" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F81" s="10" t="s">
+      <c r="E82" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F82" s="10" t="s">
         <v>443</v>
       </c>
-      <c r="G81" s="13" t="s">
+      <c r="G82" s="13" t="s">
         <v>444</v>
       </c>
-      <c r="H81" s="7">
-        <v>1</v>
-      </c>
-      <c r="I81" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J81" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K81" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="9">
-        <v>393</v>
-      </c>
-      <c r="B82" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C82" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="D82" s="12" t="s">
-        <v>264</v>
-      </c>
-      <c r="E82" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F82" s="10" t="s">
-        <v>445</v>
-      </c>
-      <c r="G82" s="13" t="s">
-        <v>446</v>
-      </c>
       <c r="H82" s="7">
         <v>1</v>
       </c>
       <c r="I82" s="14" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J82" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K82" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A83" s="9">
+        <v>393</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="D83" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F83" s="10" t="s">
+        <v>445</v>
+      </c>
+      <c r="G83" s="13" t="s">
+        <v>446</v>
+      </c>
+      <c r="H83" s="7">
+        <v>1</v>
+      </c>
+      <c r="I83" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="J83" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K83" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A84" s="9">
         <v>394</v>
       </c>
-      <c r="B83" s="10" t="s">
+      <c r="B84" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C83" s="11" t="s">
+      <c r="C84" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="D83" s="12" t="s">
+      <c r="D84" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="E83" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F83" s="10" t="s">
+      <c r="E84" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F84" s="10" t="s">
         <v>447</v>
       </c>
-      <c r="G83" s="13" t="s">
+      <c r="G84" s="13" t="s">
         <v>448</v>
       </c>
-      <c r="H83" s="7">
-        <v>1</v>
-      </c>
-      <c r="I83" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J83" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K83" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="9">
-        <v>395</v>
-      </c>
-      <c r="B84" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C84" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="D84" s="12" t="s">
-        <v>268</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F84" s="10" t="s">
-        <v>449</v>
-      </c>
-      <c r="G84" s="13" t="s">
-        <v>450</v>
-      </c>
       <c r="H84" s="7">
         <v>1</v>
       </c>
@@ -4909,33 +4886,33 @@
         <v>466</v>
       </c>
       <c r="J84" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K84" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="9">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D85" s="12" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F85" s="10" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="G85" s="13" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="H85" s="7">
         <v>1</v>
@@ -4944,104 +4921,104 @@
         <v>466</v>
       </c>
       <c r="J85" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K85" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="9">
+        <v>396</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="D86" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F86" s="10" t="s">
+        <v>451</v>
+      </c>
+      <c r="G86" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="H86" s="7">
+        <v>1</v>
+      </c>
+      <c r="I86" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="J86" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K86" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" s="9">
         <v>397</v>
       </c>
-      <c r="B86" s="10" t="s">
+      <c r="B87" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C86" s="11" t="s">
+      <c r="C87" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="D86" s="12" t="s">
+      <c r="D87" s="12" t="s">
         <v>272</v>
       </c>
-      <c r="E86" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F86" s="10" t="s">
+      <c r="E87" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F87" s="10" t="s">
         <v>453</v>
       </c>
-      <c r="G86" s="13" t="s">
+      <c r="G87" s="13" t="s">
         <v>454</v>
       </c>
-      <c r="H86" s="7">
-        <v>1</v>
-      </c>
-      <c r="I86" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J86" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K86" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="9">
+      <c r="H87" s="7">
+        <v>1</v>
+      </c>
+      <c r="I87" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="J87" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K87" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A88" s="9">
         <v>398</v>
       </c>
-      <c r="B87" s="10" t="s">
+      <c r="B88" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C87" s="11" t="s">
+      <c r="C88" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="D87" s="12" t="s">
+      <c r="D88" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="E87" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F87" s="10" t="s">
+      <c r="E88" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F88" s="10" t="s">
         <v>455</v>
       </c>
-      <c r="G87" s="13" t="s">
+      <c r="G88" s="13" t="s">
         <v>456</v>
       </c>
-      <c r="H87" s="7">
-        <v>1</v>
-      </c>
-      <c r="I87" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J87" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K87" s="15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A88" s="9">
-        <v>399</v>
-      </c>
-      <c r="B88" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C88" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="D88" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="E88" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F88" s="10" t="s">
-        <v>457</v>
-      </c>
-      <c r="G88" s="13" t="s">
-        <v>458</v>
-      </c>
       <c r="H88" s="7">
         <v>1</v>
       </c>
@@ -5049,33 +5026,33 @@
         <v>466</v>
       </c>
       <c r="J88" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K88" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D89" s="12" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F89" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="G89" s="13" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="H89" s="7">
         <v>1</v>
@@ -5084,33 +5061,33 @@
         <v>466</v>
       </c>
       <c r="J89" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K89" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D90" s="12" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F90" s="10">
-        <v>1129534717</v>
+      <c r="F90" s="10" t="s">
+        <v>459</v>
       </c>
       <c r="G90" s="13" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="H90" s="7">
         <v>1</v>
@@ -5119,33 +5096,33 @@
         <v>466</v>
       </c>
       <c r="J90" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K90" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="9">
-        <v>420</v>
+        <v>402</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D91" s="12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E91" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F91" s="10" t="s">
-        <v>462</v>
+      <c r="F91" s="10">
+        <v>1129534717</v>
       </c>
       <c r="G91" s="13" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H91" s="7">
         <v>1</v>
@@ -5154,45 +5131,80 @@
         <v>466</v>
       </c>
       <c r="J91" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K91" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="9">
+        <v>420</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C92" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="D92" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F92" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="G92" s="13" t="s">
+        <v>463</v>
+      </c>
+      <c r="H92" s="7">
+        <v>1</v>
+      </c>
+      <c r="I92" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="J92" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K92" s="15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" s="9">
         <v>422</v>
       </c>
-      <c r="B92" s="10" t="s">
+      <c r="B93" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C92" s="11" t="s">
+      <c r="C93" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="D92" s="12" t="s">
+      <c r="D93" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="E92" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F92" s="10" t="s">
+      <c r="E93" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F93" s="10" t="s">
         <v>464</v>
       </c>
-      <c r="G92" s="13" t="s">
+      <c r="G93" s="13" t="s">
         <v>465</v>
       </c>
-      <c r="H92" s="7">
-        <v>1</v>
-      </c>
-      <c r="I92" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="J92" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="K92" s="15" t="s">
-        <v>472</v>
+      <c r="H93" s="7">
+        <v>1</v>
+      </c>
+      <c r="I93" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="J93" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="K93" s="15" t="s">
+        <v>471</v>
       </c>
     </row>
   </sheetData>

</xml_diff>